<commit_message>
Updated on 10 July 2022
</commit_message>
<xml_diff>
--- a/20220708_matching.xlsx
+++ b/20220708_matching.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofnottm-my.sharepoint.com/personal/arif_sulistiono_nottingham_ac_uk/Documents/BB_SideProject/BelutListrik/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="318" documentId="11_C424699D9CC787E287F4BBC68128670D4D019EB9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C1E14DC-E675-7E49-8AC7-12F43C4D09C0}"/>
+  <xr:revisionPtr revIDLastSave="320" documentId="11_C424699D9CC787E287F4BBC68128670D4D019EB9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECD65B58-C1A4-BB48-8A31-51659CD73A9D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3095,10 +3095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J721"/>
+  <dimension ref="A1:J720"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A581" workbookViewId="0">
+      <selection activeCell="L606" sqref="L606"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18066,6 +18066,18 @@
       <c r="F601" t="s">
         <v>548</v>
       </c>
+      <c r="G601" t="s">
+        <v>775</v>
+      </c>
+      <c r="H601" t="s">
+        <v>556</v>
+      </c>
+      <c r="I601">
+        <v>262</v>
+      </c>
+      <c r="J601" t="s">
+        <v>893</v>
+      </c>
     </row>
     <row r="602" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A602" t="s">
@@ -18101,87 +18113,93 @@
     </row>
     <row r="603" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G603" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="H603" t="s">
-        <v>556</v>
+        <v>815</v>
       </c>
       <c r="I603">
-        <v>262</v>
+        <v>427</v>
       </c>
       <c r="J603" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
     </row>
     <row r="604" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G604" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="H604" t="s">
         <v>815</v>
       </c>
       <c r="I604">
-        <v>427</v>
+        <v>2</v>
       </c>
       <c r="J604" t="s">
-        <v>894</v>
+        <v>777</v>
       </c>
     </row>
     <row r="605" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A605" t="s">
+        <v>231</v>
+      </c>
+      <c r="B605" t="s">
+        <v>521</v>
+      </c>
+      <c r="C605">
+        <v>3</v>
+      </c>
+      <c r="D605" t="s">
+        <v>532</v>
+      </c>
+      <c r="E605">
+        <v>4</v>
+      </c>
+      <c r="F605" t="s">
+        <v>545</v>
+      </c>
       <c r="G605" t="s">
-        <v>777</v>
+        <v>231</v>
       </c>
       <c r="H605" t="s">
-        <v>815</v>
+        <v>556</v>
       </c>
       <c r="I605">
-        <v>2</v>
+        <v>473</v>
       </c>
       <c r="J605" t="s">
-        <v>777</v>
+        <v>231</v>
       </c>
     </row>
     <row r="606" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A606" t="s">
-        <v>231</v>
+        <v>74</v>
       </c>
       <c r="B606" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="C606">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D606" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="E606">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="F606" t="s">
-        <v>545</v>
-      </c>
-      <c r="G606" t="s">
-        <v>231</v>
-      </c>
-      <c r="H606" t="s">
-        <v>556</v>
-      </c>
-      <c r="I606">
-        <v>473</v>
-      </c>
-      <c r="J606" t="s">
-        <v>231</v>
+        <v>538</v>
       </c>
     </row>
     <row r="607" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A607" t="s">
-        <v>74</v>
+        <v>374</v>
       </c>
       <c r="B607" t="s">
-        <v>514</v>
+        <v>526</v>
       </c>
       <c r="C607">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D607" t="s">
         <v>534</v>
@@ -18190,50 +18208,62 @@
         <v>5.5</v>
       </c>
       <c r="F607" t="s">
-        <v>538</v>
+        <v>550</v>
+      </c>
+      <c r="G607" t="s">
+        <v>374</v>
+      </c>
+      <c r="H607" t="s">
+        <v>557</v>
+      </c>
+      <c r="I607">
+        <v>298</v>
+      </c>
+      <c r="J607" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="608" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A608" t="s">
-        <v>374</v>
+        <v>64</v>
       </c>
       <c r="B608" t="s">
-        <v>526</v>
+        <v>514</v>
       </c>
       <c r="C608">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D608" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E608">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="F608" t="s">
-        <v>550</v>
+        <v>538</v>
       </c>
       <c r="G608" t="s">
-        <v>374</v>
+        <v>64</v>
       </c>
       <c r="H608" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I608">
-        <v>298</v>
+        <v>415</v>
       </c>
       <c r="J608" t="s">
-        <v>374</v>
+        <v>64</v>
       </c>
     </row>
     <row r="609" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A609" t="s">
-        <v>64</v>
+        <v>452</v>
       </c>
       <c r="B609" t="s">
-        <v>514</v>
+        <v>529</v>
       </c>
       <c r="C609">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D609" t="s">
         <v>532</v>
@@ -18242,1383 +18272,1383 @@
         <v>4.5</v>
       </c>
       <c r="F609" t="s">
-        <v>538</v>
+        <v>553</v>
       </c>
       <c r="G609" t="s">
-        <v>64</v>
+        <v>452</v>
       </c>
       <c r="H609" t="s">
         <v>556</v>
       </c>
       <c r="I609">
-        <v>415</v>
+        <v>368</v>
       </c>
       <c r="J609" t="s">
-        <v>64</v>
+        <v>452</v>
       </c>
     </row>
     <row r="610" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A610" t="s">
-        <v>452</v>
+        <v>402</v>
       </c>
       <c r="B610" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C610">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D610" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="E610">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="F610" t="s">
-        <v>553</v>
-      </c>
-      <c r="G610" t="s">
-        <v>452</v>
-      </c>
-      <c r="H610" t="s">
-        <v>556</v>
-      </c>
-      <c r="I610">
-        <v>368</v>
-      </c>
-      <c r="J610" t="s">
-        <v>452</v>
+        <v>551</v>
       </c>
     </row>
     <row r="611" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A611" t="s">
-        <v>402</v>
-      </c>
-      <c r="B611" t="s">
-        <v>527</v>
-      </c>
-      <c r="C611">
-        <v>2</v>
-      </c>
-      <c r="D611" t="s">
+      <c r="G611" t="s">
+        <v>778</v>
+      </c>
+      <c r="H611" t="s">
+        <v>557</v>
+      </c>
+      <c r="I611">
+        <v>230</v>
+      </c>
+      <c r="J611" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="612" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A612" t="s">
+        <v>480</v>
+      </c>
+      <c r="B612" t="s">
+        <v>530</v>
+      </c>
+      <c r="C612">
+        <v>3</v>
+      </c>
+      <c r="D612" t="s">
         <v>534</v>
       </c>
-      <c r="E611">
-        <v>5</v>
-      </c>
-      <c r="F611" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="612" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E612">
+        <v>6</v>
+      </c>
+      <c r="F612" t="s">
+        <v>554</v>
+      </c>
       <c r="G612" t="s">
-        <v>778</v>
+        <v>480</v>
       </c>
       <c r="H612" t="s">
         <v>557</v>
       </c>
       <c r="I612">
-        <v>230</v>
+        <v>419</v>
       </c>
       <c r="J612" t="s">
-        <v>778</v>
+        <v>895</v>
       </c>
     </row>
     <row r="613" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A613" t="s">
-        <v>480</v>
+        <v>185</v>
       </c>
       <c r="B613" t="s">
-        <v>530</v>
+        <v>519</v>
       </c>
       <c r="C613">
         <v>3</v>
       </c>
       <c r="D613" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="E613">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F613" t="s">
-        <v>554</v>
+        <v>543</v>
       </c>
       <c r="G613" t="s">
-        <v>480</v>
+        <v>185</v>
       </c>
       <c r="H613" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="I613">
-        <v>419</v>
+        <v>591</v>
       </c>
       <c r="J613" t="s">
-        <v>895</v>
+        <v>185</v>
       </c>
     </row>
     <row r="614" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A614" t="s">
-        <v>185</v>
-      </c>
-      <c r="B614" t="s">
-        <v>519</v>
-      </c>
-      <c r="C614">
-        <v>3</v>
-      </c>
-      <c r="D614" t="s">
+      <c r="G614" t="s">
+        <v>779</v>
+      </c>
+      <c r="H614" t="s">
+        <v>556</v>
+      </c>
+      <c r="I614">
+        <v>321</v>
+      </c>
+      <c r="J614" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="615" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A615" t="s">
+        <v>271</v>
+      </c>
+      <c r="B615" t="s">
+        <v>522</v>
+      </c>
+      <c r="C615">
+        <v>2</v>
+      </c>
+      <c r="D615" t="s">
         <v>535</v>
       </c>
-      <c r="E614">
-        <v>5</v>
-      </c>
-      <c r="F614" t="s">
-        <v>543</v>
-      </c>
-      <c r="G614" t="s">
-        <v>185</v>
-      </c>
-      <c r="H614" t="s">
+      <c r="E615">
+        <v>4.5</v>
+      </c>
+      <c r="F615" t="s">
+        <v>546</v>
+      </c>
+      <c r="G615" t="s">
+        <v>271</v>
+      </c>
+      <c r="H615" t="s">
         <v>558</v>
       </c>
-      <c r="I614">
-        <v>591</v>
-      </c>
-      <c r="J614" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="615" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G615" t="s">
-        <v>779</v>
-      </c>
-      <c r="H615" t="s">
-        <v>556</v>
-      </c>
       <c r="I615">
-        <v>321</v>
+        <v>550</v>
       </c>
       <c r="J615" t="s">
-        <v>779</v>
+        <v>271</v>
       </c>
     </row>
     <row r="616" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A616" t="s">
-        <v>271</v>
+        <v>181</v>
       </c>
       <c r="B616" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C616">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D616" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E616">
         <v>4.5</v>
       </c>
       <c r="F616" t="s">
-        <v>546</v>
-      </c>
-      <c r="G616" t="s">
-        <v>271</v>
-      </c>
-      <c r="H616" t="s">
-        <v>558</v>
-      </c>
-      <c r="I616">
-        <v>550</v>
-      </c>
-      <c r="J616" t="s">
-        <v>271</v>
+        <v>542</v>
       </c>
     </row>
     <row r="617" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A617" t="s">
-        <v>181</v>
+        <v>406</v>
       </c>
       <c r="B617" t="s">
-        <v>518</v>
+        <v>527</v>
       </c>
       <c r="C617">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D617" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="E617">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="F617" t="s">
-        <v>542</v>
+        <v>551</v>
       </c>
     </row>
     <row r="618" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A618" t="s">
-        <v>406</v>
+        <v>93</v>
       </c>
       <c r="B618" t="s">
-        <v>527</v>
+        <v>515</v>
       </c>
       <c r="C618">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D618" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E618">
         <v>5</v>
       </c>
       <c r="F618" t="s">
-        <v>551</v>
+        <v>539</v>
+      </c>
+      <c r="G618" t="s">
+        <v>93</v>
+      </c>
+      <c r="H618" t="s">
+        <v>557</v>
+      </c>
+      <c r="I618">
+        <v>85</v>
+      </c>
+      <c r="J618" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="619" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A619" t="s">
-        <v>93</v>
-      </c>
-      <c r="B619" t="s">
-        <v>515</v>
-      </c>
-      <c r="C619">
-        <v>3</v>
-      </c>
-      <c r="D619" t="s">
-        <v>534</v>
-      </c>
-      <c r="E619">
-        <v>5</v>
-      </c>
-      <c r="F619" t="s">
-        <v>539</v>
-      </c>
       <c r="G619" t="s">
-        <v>93</v>
+        <v>780</v>
       </c>
       <c r="H619" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I619">
-        <v>85</v>
+        <v>677</v>
       </c>
       <c r="J619" t="s">
-        <v>93</v>
+        <v>896</v>
       </c>
     </row>
     <row r="620" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G620" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="H620" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="I620">
-        <v>677</v>
+        <v>698</v>
       </c>
       <c r="J620" t="s">
-        <v>896</v>
+        <v>781</v>
       </c>
     </row>
     <row r="621" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G621" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="H621" t="s">
         <v>557</v>
       </c>
       <c r="I621">
-        <v>698</v>
+        <v>592</v>
       </c>
       <c r="J621" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="622" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A622" t="s">
+        <v>339</v>
+      </c>
+      <c r="B622" t="s">
+        <v>524</v>
+      </c>
+      <c r="C622">
+        <v>5</v>
+      </c>
+      <c r="D622" t="s">
+        <v>533</v>
+      </c>
+      <c r="E622">
+        <v>4</v>
+      </c>
+      <c r="F622" t="s">
+        <v>548</v>
+      </c>
       <c r="G622" t="s">
-        <v>782</v>
+        <v>339</v>
       </c>
       <c r="H622" t="s">
-        <v>557</v>
+        <v>815</v>
       </c>
       <c r="I622">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="J622" t="s">
-        <v>782</v>
+        <v>339</v>
       </c>
     </row>
     <row r="623" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A623" t="s">
-        <v>339</v>
+        <v>400</v>
       </c>
       <c r="B623" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="C623">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D623" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E623">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="F623" t="s">
-        <v>548</v>
-      </c>
-      <c r="G623" t="s">
-        <v>339</v>
-      </c>
-      <c r="H623" t="s">
-        <v>815</v>
-      </c>
-      <c r="I623">
-        <v>593</v>
-      </c>
-      <c r="J623" t="s">
-        <v>339</v>
+        <v>551</v>
       </c>
     </row>
     <row r="624" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A624" t="s">
-        <v>400</v>
+        <v>352</v>
       </c>
       <c r="B624" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C624">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D624" t="s">
+        <v>534</v>
+      </c>
+      <c r="E624">
+        <v>5</v>
+      </c>
+      <c r="F624" t="s">
+        <v>549</v>
+      </c>
+      <c r="G624" t="s">
+        <v>352</v>
+      </c>
+      <c r="H624" t="s">
+        <v>557</v>
+      </c>
+      <c r="I624">
+        <v>285</v>
+      </c>
+      <c r="J624" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="625" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G625" t="s">
+        <v>783</v>
+      </c>
+      <c r="H625" t="s">
+        <v>556</v>
+      </c>
+      <c r="I625">
+        <v>11</v>
+      </c>
+      <c r="J625" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="626" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A626" t="s">
+        <v>186</v>
+      </c>
+      <c r="B626" t="s">
+        <v>519</v>
+      </c>
+      <c r="C626">
+        <v>3</v>
+      </c>
+      <c r="D626" t="s">
         <v>532</v>
       </c>
-      <c r="E624">
+      <c r="E626">
         <v>4.5</v>
       </c>
-      <c r="F624" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="625" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A625" t="s">
-        <v>352</v>
-      </c>
-      <c r="B625" t="s">
-        <v>525</v>
-      </c>
-      <c r="C625">
-        <v>4</v>
-      </c>
-      <c r="D625" t="s">
-        <v>534</v>
-      </c>
-      <c r="E625">
-        <v>5</v>
-      </c>
-      <c r="F625" t="s">
-        <v>549</v>
-      </c>
-      <c r="G625" t="s">
-        <v>352</v>
-      </c>
-      <c r="H625" t="s">
-        <v>557</v>
-      </c>
-      <c r="I625">
-        <v>285</v>
-      </c>
-      <c r="J625" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="626" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F626" t="s">
+        <v>543</v>
+      </c>
       <c r="G626" t="s">
-        <v>783</v>
+        <v>186</v>
       </c>
       <c r="H626" t="s">
         <v>556</v>
       </c>
       <c r="I626">
-        <v>11</v>
+        <v>165</v>
       </c>
       <c r="J626" t="s">
-        <v>783</v>
+        <v>186</v>
       </c>
     </row>
     <row r="627" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A627" t="s">
-        <v>186</v>
+        <v>385</v>
       </c>
       <c r="B627" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="C627">
         <v>3</v>
       </c>
       <c r="D627" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="E627">
         <v>4.5</v>
       </c>
       <c r="F627" t="s">
-        <v>543</v>
+        <v>550</v>
       </c>
       <c r="G627" t="s">
-        <v>186</v>
+        <v>385</v>
       </c>
       <c r="H627" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="I627">
-        <v>165</v>
+        <v>309</v>
       </c>
       <c r="J627" t="s">
-        <v>186</v>
+        <v>385</v>
       </c>
     </row>
     <row r="628" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A628" t="s">
-        <v>385</v>
+        <v>311</v>
       </c>
       <c r="B628" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="C628">
+        <v>5</v>
+      </c>
+      <c r="D628" t="s">
+        <v>532</v>
+      </c>
+      <c r="E628">
+        <v>4</v>
+      </c>
+      <c r="F628" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="629" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G629" t="s">
+        <v>784</v>
+      </c>
+      <c r="H629" t="s">
+        <v>556</v>
+      </c>
+      <c r="I629">
+        <v>358</v>
+      </c>
+      <c r="J629" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="630" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A630" t="s">
+        <v>88</v>
+      </c>
+      <c r="B630" t="s">
+        <v>515</v>
+      </c>
+      <c r="C630">
         <v>3</v>
       </c>
-      <c r="D628" t="s">
-        <v>534</v>
-      </c>
-      <c r="E628">
-        <v>4.5</v>
-      </c>
-      <c r="F628" t="s">
-        <v>550</v>
-      </c>
-      <c r="G628" t="s">
-        <v>385</v>
-      </c>
-      <c r="H628" t="s">
-        <v>557</v>
-      </c>
-      <c r="I628">
-        <v>309</v>
-      </c>
-      <c r="J628" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="629" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A629" t="s">
-        <v>311</v>
-      </c>
-      <c r="B629" t="s">
-        <v>523</v>
-      </c>
-      <c r="C629">
+      <c r="D630" t="s">
+        <v>532</v>
+      </c>
+      <c r="E630">
         <v>5</v>
       </c>
-      <c r="D629" t="s">
-        <v>532</v>
-      </c>
-      <c r="E629">
-        <v>4</v>
-      </c>
-      <c r="F629" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="630" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F630" t="s">
+        <v>539</v>
+      </c>
       <c r="G630" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="H630" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="I630">
-        <v>358</v>
+        <v>81</v>
       </c>
       <c r="J630" t="s">
-        <v>784</v>
+        <v>897</v>
       </c>
     </row>
     <row r="631" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A631" t="s">
-        <v>88</v>
+        <v>454</v>
       </c>
       <c r="B631" t="s">
-        <v>515</v>
+        <v>529</v>
       </c>
       <c r="C631">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D631" t="s">
         <v>532</v>
       </c>
       <c r="E631">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="F631" t="s">
-        <v>539</v>
+        <v>553</v>
       </c>
       <c r="G631" t="s">
-        <v>785</v>
+        <v>454</v>
       </c>
       <c r="H631" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I631">
-        <v>81</v>
+        <v>370</v>
       </c>
       <c r="J631" t="s">
-        <v>897</v>
+        <v>454</v>
       </c>
     </row>
     <row r="632" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A632" t="s">
-        <v>454</v>
+        <v>100</v>
       </c>
       <c r="B632" t="s">
-        <v>529</v>
+        <v>515</v>
       </c>
       <c r="C632">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D632" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="E632">
         <v>4.5</v>
       </c>
       <c r="F632" t="s">
-        <v>553</v>
+        <v>539</v>
       </c>
       <c r="G632" t="s">
-        <v>454</v>
+        <v>100</v>
       </c>
       <c r="H632" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="I632">
-        <v>370</v>
+        <v>499</v>
       </c>
       <c r="J632" t="s">
-        <v>454</v>
+        <v>100</v>
       </c>
     </row>
     <row r="633" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A633" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="B633" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C633">
         <v>3</v>
       </c>
       <c r="D633" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E633">
         <v>4.5</v>
       </c>
       <c r="F633" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="G633" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="H633" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I633">
-        <v>499</v>
+        <v>56</v>
       </c>
       <c r="J633" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
     </row>
     <row r="634" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A634" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="B634" t="s">
+        <v>514</v>
+      </c>
+      <c r="C634">
+        <v>2</v>
+      </c>
+      <c r="D634" t="s">
+        <v>534</v>
+      </c>
+      <c r="E634">
+        <v>5</v>
+      </c>
+      <c r="F634" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="635" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G635" t="s">
+        <v>786</v>
+      </c>
+      <c r="H635" t="s">
+        <v>558</v>
+      </c>
+      <c r="I635">
+        <v>519</v>
+      </c>
+      <c r="J635" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="636" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A636" t="s">
+        <v>113</v>
+      </c>
+      <c r="B636" t="s">
         <v>516</v>
       </c>
-      <c r="C634">
+      <c r="C636">
         <v>3</v>
       </c>
-      <c r="D634" t="s">
-        <v>532</v>
-      </c>
-      <c r="E634">
-        <v>4.5</v>
-      </c>
-      <c r="F634" t="s">
+      <c r="D636" t="s">
+        <v>534</v>
+      </c>
+      <c r="E636">
+        <v>5</v>
+      </c>
+      <c r="F636" t="s">
         <v>540</v>
       </c>
-      <c r="G634" t="s">
-        <v>111</v>
-      </c>
-      <c r="H634" t="s">
-        <v>556</v>
-      </c>
-      <c r="I634">
-        <v>56</v>
-      </c>
-      <c r="J634" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="635" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A635" t="s">
-        <v>79</v>
-      </c>
-      <c r="B635" t="s">
-        <v>514</v>
-      </c>
-      <c r="C635">
-        <v>2</v>
-      </c>
-      <c r="D635" t="s">
-        <v>534</v>
-      </c>
-      <c r="E635">
-        <v>5</v>
-      </c>
-      <c r="F635" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="636" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G636" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="H636" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I636">
-        <v>519</v>
+        <v>727</v>
       </c>
       <c r="J636" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
     </row>
     <row r="637" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A637" t="s">
-        <v>113</v>
+        <v>337</v>
       </c>
       <c r="B637" t="s">
-        <v>516</v>
+        <v>524</v>
       </c>
       <c r="C637">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D637" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E637">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F637" t="s">
-        <v>540</v>
-      </c>
-      <c r="G637" t="s">
-        <v>787</v>
-      </c>
-      <c r="H637" t="s">
-        <v>557</v>
-      </c>
-      <c r="I637">
-        <v>727</v>
-      </c>
-      <c r="J637" t="s">
-        <v>787</v>
+        <v>548</v>
       </c>
     </row>
     <row r="638" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A638" t="s">
-        <v>337</v>
+        <v>394</v>
       </c>
       <c r="B638" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="C638">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D638" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E638">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="F638" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="639" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A639" t="s">
-        <v>394</v>
-      </c>
-      <c r="B639" t="s">
-        <v>527</v>
-      </c>
-      <c r="C639">
-        <v>2</v>
-      </c>
-      <c r="D639" t="s">
-        <v>532</v>
-      </c>
-      <c r="E639">
-        <v>4.5</v>
-      </c>
-      <c r="F639" t="s">
-        <v>551</v>
+      <c r="G639" t="s">
+        <v>788</v>
+      </c>
+      <c r="H639" t="s">
+        <v>557</v>
+      </c>
+      <c r="I639">
+        <v>60</v>
+      </c>
+      <c r="J639" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="640" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G640" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="H640" t="s">
         <v>557</v>
       </c>
       <c r="I640">
-        <v>60</v>
+        <v>634</v>
       </c>
       <c r="J640" t="s">
-        <v>113</v>
+        <v>789</v>
       </c>
     </row>
     <row r="641" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A641" t="s">
+        <v>121</v>
+      </c>
+      <c r="B641" t="s">
+        <v>516</v>
+      </c>
+      <c r="C641">
+        <v>3</v>
+      </c>
+      <c r="D641" t="s">
+        <v>534</v>
+      </c>
+      <c r="E641">
+        <v>4.5</v>
+      </c>
+      <c r="F641" t="s">
+        <v>540</v>
+      </c>
       <c r="G641" t="s">
-        <v>789</v>
+        <v>121</v>
       </c>
       <c r="H641" t="s">
         <v>557</v>
       </c>
       <c r="I641">
-        <v>634</v>
+        <v>73</v>
       </c>
       <c r="J641" t="s">
-        <v>789</v>
+        <v>121</v>
       </c>
     </row>
     <row r="642" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A642" t="s">
-        <v>121</v>
+        <v>453</v>
       </c>
       <c r="B642" t="s">
-        <v>516</v>
+        <v>529</v>
       </c>
       <c r="C642">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D642" t="s">
         <v>534</v>
       </c>
       <c r="E642">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="F642" t="s">
-        <v>540</v>
+        <v>553</v>
       </c>
       <c r="G642" t="s">
-        <v>121</v>
+        <v>453</v>
       </c>
       <c r="H642" t="s">
         <v>557</v>
       </c>
       <c r="I642">
-        <v>73</v>
+        <v>369</v>
       </c>
       <c r="J642" t="s">
-        <v>121</v>
+        <v>453</v>
       </c>
     </row>
     <row r="643" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A643" t="s">
-        <v>453</v>
-      </c>
-      <c r="B643" t="s">
-        <v>529</v>
-      </c>
-      <c r="C643">
-        <v>4</v>
-      </c>
-      <c r="D643" t="s">
+      <c r="G643" t="s">
+        <v>790</v>
+      </c>
+      <c r="H643" t="s">
+        <v>558</v>
+      </c>
+      <c r="I643">
+        <v>388</v>
+      </c>
+      <c r="J643" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="644" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A644" t="s">
+        <v>422</v>
+      </c>
+      <c r="B644" t="s">
+        <v>528</v>
+      </c>
+      <c r="C644">
+        <v>3</v>
+      </c>
+      <c r="D644" t="s">
         <v>534</v>
       </c>
-      <c r="E643">
-        <v>5.5</v>
-      </c>
-      <c r="F643" t="s">
-        <v>553</v>
-      </c>
-      <c r="G643" t="s">
-        <v>453</v>
-      </c>
-      <c r="H643" t="s">
-        <v>557</v>
-      </c>
-      <c r="I643">
-        <v>369</v>
-      </c>
-      <c r="J643" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="644" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E644">
+        <v>5</v>
+      </c>
+      <c r="F644" t="s">
+        <v>552</v>
+      </c>
       <c r="G644" t="s">
-        <v>790</v>
+        <v>422</v>
       </c>
       <c r="H644" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I644">
-        <v>388</v>
+        <v>339</v>
       </c>
       <c r="J644" t="s">
-        <v>790</v>
+        <v>422</v>
       </c>
     </row>
     <row r="645" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A645" t="s">
-        <v>422</v>
+        <v>260</v>
       </c>
       <c r="B645" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="C645">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D645" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E645">
         <v>5</v>
       </c>
       <c r="F645" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="G645" t="s">
-        <v>422</v>
+        <v>260</v>
       </c>
       <c r="H645" t="s">
         <v>557</v>
       </c>
       <c r="I645">
-        <v>339</v>
+        <v>188</v>
       </c>
       <c r="J645" t="s">
-        <v>422</v>
+        <v>260</v>
       </c>
     </row>
     <row r="646" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A646" t="s">
-        <v>260</v>
+        <v>392</v>
       </c>
       <c r="B646" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="C646">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D646" t="s">
         <v>532</v>
       </c>
       <c r="E646">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="F646" t="s">
-        <v>546</v>
-      </c>
-      <c r="G646" t="s">
-        <v>260</v>
-      </c>
-      <c r="H646" t="s">
-        <v>557</v>
-      </c>
-      <c r="I646">
-        <v>188</v>
-      </c>
-      <c r="J646" t="s">
-        <v>260</v>
+        <v>550</v>
       </c>
     </row>
     <row r="647" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A647" t="s">
-        <v>392</v>
-      </c>
-      <c r="B647" t="s">
-        <v>526</v>
-      </c>
-      <c r="C647">
-        <v>3</v>
-      </c>
-      <c r="D647" t="s">
-        <v>532</v>
-      </c>
-      <c r="E647">
-        <v>4.5</v>
-      </c>
-      <c r="F647" t="s">
-        <v>550</v>
+      <c r="G647" t="s">
+        <v>791</v>
+      </c>
+      <c r="H647" t="s">
+        <v>557</v>
+      </c>
+      <c r="I647">
+        <v>601</v>
+      </c>
+      <c r="J647" t="s">
+        <v>791</v>
       </c>
     </row>
     <row r="648" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G648" t="s">
-        <v>791</v>
-      </c>
-      <c r="H648" t="s">
-        <v>557</v>
-      </c>
-      <c r="I648">
-        <v>601</v>
-      </c>
-      <c r="J648" t="s">
-        <v>791</v>
+      <c r="A648" t="s">
+        <v>412</v>
+      </c>
+      <c r="B648" t="s">
+        <v>527</v>
+      </c>
+      <c r="C648">
+        <v>2</v>
+      </c>
+      <c r="D648" t="s">
+        <v>535</v>
+      </c>
+      <c r="E648">
+        <v>6</v>
+      </c>
+      <c r="F648" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="649" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A649" t="s">
-        <v>412</v>
+        <v>19</v>
       </c>
       <c r="B649" t="s">
-        <v>527</v>
+        <v>512</v>
       </c>
       <c r="C649">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D649" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="E649">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="F649" t="s">
-        <v>551</v>
+        <v>536</v>
+      </c>
+      <c r="G649" t="s">
+        <v>19</v>
+      </c>
+      <c r="H649" t="s">
+        <v>556</v>
+      </c>
+      <c r="I649">
+        <v>590</v>
+      </c>
+      <c r="J649" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="650" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A650" t="s">
-        <v>19</v>
-      </c>
-      <c r="B650" t="s">
-        <v>512</v>
-      </c>
-      <c r="C650">
-        <v>4</v>
-      </c>
-      <c r="D650" t="s">
-        <v>532</v>
-      </c>
-      <c r="E650">
-        <v>4.5</v>
-      </c>
-      <c r="F650" t="s">
-        <v>536</v>
-      </c>
       <c r="G650" t="s">
-        <v>19</v>
+        <v>792</v>
       </c>
       <c r="H650" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="I650">
-        <v>590</v>
+        <v>236</v>
       </c>
       <c r="J650" t="s">
-        <v>19</v>
+        <v>792</v>
       </c>
     </row>
     <row r="651" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G651" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="H651" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="I651">
-        <v>236</v>
+        <v>136</v>
       </c>
       <c r="J651" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
     </row>
     <row r="652" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G652" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="H652" t="s">
+        <v>557</v>
+      </c>
+      <c r="I652">
+        <v>375</v>
+      </c>
+      <c r="J652" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="653" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A653" t="s">
+        <v>120</v>
+      </c>
+      <c r="B653" t="s">
+        <v>516</v>
+      </c>
+      <c r="C653">
+        <v>3</v>
+      </c>
+      <c r="D653" t="s">
+        <v>532</v>
+      </c>
+      <c r="E653">
+        <v>4.5</v>
+      </c>
+      <c r="F653" t="s">
+        <v>540</v>
+      </c>
+      <c r="G653" t="s">
+        <v>120</v>
+      </c>
+      <c r="H653" t="s">
+        <v>556</v>
+      </c>
+      <c r="I653">
+        <v>71</v>
+      </c>
+      <c r="J653" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="654" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G654" t="s">
+        <v>795</v>
+      </c>
+      <c r="H654" t="s">
+        <v>557</v>
+      </c>
+      <c r="I654">
+        <v>79</v>
+      </c>
+      <c r="J654" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="655" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A655" t="s">
+        <v>127</v>
+      </c>
+      <c r="B655" t="s">
+        <v>516</v>
+      </c>
+      <c r="C655">
+        <v>3</v>
+      </c>
+      <c r="D655" t="s">
+        <v>534</v>
+      </c>
+      <c r="E655">
+        <v>4.5</v>
+      </c>
+      <c r="F655" t="s">
+        <v>540</v>
+      </c>
+      <c r="G655" t="s">
+        <v>127</v>
+      </c>
+      <c r="H655" t="s">
+        <v>557</v>
+      </c>
+      <c r="I655">
+        <v>537</v>
+      </c>
+      <c r="J655" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="656" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G656" t="s">
+        <v>796</v>
+      </c>
+      <c r="H656" t="s">
         <v>558</v>
       </c>
-      <c r="I652">
-        <v>136</v>
-      </c>
-      <c r="J652" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="653" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G653" t="s">
-        <v>794</v>
-      </c>
-      <c r="H653" t="s">
-        <v>557</v>
-      </c>
-      <c r="I653">
-        <v>375</v>
-      </c>
-      <c r="J653" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="654" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A654" t="s">
-        <v>120</v>
-      </c>
-      <c r="B654" t="s">
-        <v>516</v>
-      </c>
-      <c r="C654">
-        <v>3</v>
-      </c>
-      <c r="D654" t="s">
+      <c r="I656">
+        <v>315</v>
+      </c>
+      <c r="J656" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="657" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A657" t="s">
+        <v>216</v>
+      </c>
+      <c r="B657" t="s">
+        <v>520</v>
+      </c>
+      <c r="C657">
+        <v>2</v>
+      </c>
+      <c r="D657" t="s">
         <v>532</v>
       </c>
-      <c r="E654">
-        <v>4.5</v>
-      </c>
-      <c r="F654" t="s">
-        <v>540</v>
-      </c>
-      <c r="G654" t="s">
-        <v>120</v>
-      </c>
-      <c r="H654" t="s">
-        <v>556</v>
-      </c>
-      <c r="I654">
-        <v>71</v>
-      </c>
-      <c r="J654" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="655" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G655" t="s">
-        <v>795</v>
-      </c>
-      <c r="H655" t="s">
-        <v>557</v>
-      </c>
-      <c r="I655">
-        <v>79</v>
-      </c>
-      <c r="J655" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="656" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A656" t="s">
-        <v>127</v>
-      </c>
-      <c r="B656" t="s">
-        <v>516</v>
-      </c>
-      <c r="C656">
-        <v>3</v>
-      </c>
-      <c r="D656" t="s">
-        <v>534</v>
-      </c>
-      <c r="E656">
-        <v>4.5</v>
-      </c>
-      <c r="F656" t="s">
-        <v>540</v>
-      </c>
-      <c r="G656" t="s">
-        <v>127</v>
-      </c>
-      <c r="H656" t="s">
-        <v>557</v>
-      </c>
-      <c r="I656">
-        <v>537</v>
-      </c>
-      <c r="J656" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="657" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G657" t="s">
-        <v>796</v>
-      </c>
-      <c r="H657" t="s">
-        <v>558</v>
-      </c>
-      <c r="I657">
-        <v>315</v>
-      </c>
-      <c r="J657" t="s">
-        <v>796</v>
+      <c r="E657">
+        <v>4</v>
+      </c>
+      <c r="F657" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="658" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A658" t="s">
-        <v>216</v>
+        <v>417</v>
       </c>
       <c r="B658" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
       <c r="C658">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D658" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="E658">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F658" t="s">
-        <v>544</v>
+        <v>552</v>
+      </c>
+      <c r="G658" t="s">
+        <v>417</v>
+      </c>
+      <c r="H658" t="s">
+        <v>557</v>
+      </c>
+      <c r="I658">
+        <v>332</v>
+      </c>
+      <c r="J658" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="659" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A659" t="s">
-        <v>417</v>
+        <v>286</v>
       </c>
       <c r="B659" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="C659">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D659" t="s">
         <v>534</v>
       </c>
       <c r="E659">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="F659" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="G659" t="s">
-        <v>417</v>
+        <v>286</v>
       </c>
       <c r="H659" t="s">
         <v>557</v>
       </c>
       <c r="I659">
-        <v>332</v>
+        <v>225</v>
       </c>
       <c r="J659" t="s">
-        <v>417</v>
+        <v>899</v>
       </c>
     </row>
     <row r="660" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A660" t="s">
-        <v>286</v>
+        <v>134</v>
       </c>
       <c r="B660" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="C660">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D660" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E660">
         <v>5.5</v>
       </c>
       <c r="F660" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="G660" t="s">
-        <v>286</v>
+        <v>134</v>
       </c>
       <c r="H660" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I660">
-        <v>225</v>
+        <v>121</v>
       </c>
       <c r="J660" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
     </row>
     <row r="661" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A661" t="s">
-        <v>134</v>
+        <v>11</v>
       </c>
       <c r="B661" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="C661">
         <v>4</v>
       </c>
       <c r="D661" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="E661">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="F661" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="G661" t="s">
-        <v>134</v>
+        <v>11</v>
       </c>
       <c r="H661" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="I661">
-        <v>121</v>
+        <v>15</v>
       </c>
       <c r="J661" t="s">
-        <v>900</v>
+        <v>11</v>
       </c>
     </row>
     <row r="662" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A662" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="B662" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C662">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D662" t="s">
         <v>534</v>
       </c>
       <c r="E662">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="F662" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="G662" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="H662" t="s">
         <v>557</v>
       </c>
       <c r="I662">
-        <v>15</v>
+        <v>638</v>
       </c>
       <c r="J662" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
     </row>
     <row r="663" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A663" t="s">
-        <v>54</v>
+        <v>209</v>
       </c>
       <c r="B663" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="C663">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D663" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E663">
         <v>4.5</v>
       </c>
       <c r="F663" t="s">
-        <v>537</v>
-      </c>
-      <c r="G663" t="s">
-        <v>54</v>
-      </c>
-      <c r="H663" t="s">
-        <v>557</v>
-      </c>
-      <c r="I663">
-        <v>638</v>
-      </c>
-      <c r="J663" t="s">
-        <v>54</v>
+        <v>544</v>
       </c>
     </row>
     <row r="664" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A664" t="s">
-        <v>209</v>
-      </c>
-      <c r="B664" t="s">
-        <v>520</v>
-      </c>
-      <c r="C664">
-        <v>2</v>
-      </c>
-      <c r="D664" t="s">
-        <v>532</v>
-      </c>
-      <c r="E664">
-        <v>4.5</v>
-      </c>
-      <c r="F664" t="s">
-        <v>544</v>
+      <c r="G664" t="s">
+        <v>797</v>
+      </c>
+      <c r="H664" t="s">
+        <v>815</v>
+      </c>
+      <c r="I664">
+        <v>314</v>
+      </c>
+      <c r="J664" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="665" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A665" t="s">
+        <v>143</v>
+      </c>
+      <c r="B665" t="s">
+        <v>517</v>
+      </c>
+      <c r="C665">
+        <v>4</v>
+      </c>
+      <c r="D665" t="s">
+        <v>535</v>
+      </c>
+      <c r="E665">
+        <v>8</v>
+      </c>
+      <c r="F665" t="s">
+        <v>541</v>
+      </c>
       <c r="G665" t="s">
-        <v>797</v>
+        <v>143</v>
       </c>
       <c r="H665" t="s">
-        <v>815</v>
+        <v>558</v>
       </c>
       <c r="I665">
-        <v>314</v>
+        <v>134</v>
       </c>
       <c r="J665" t="s">
-        <v>797</v>
+        <v>143</v>
       </c>
     </row>
     <row r="666" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A666" t="s">
-        <v>143</v>
+        <v>239</v>
       </c>
       <c r="B666" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="C666">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D666" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="E666">
-        <v>8</v>
+        <v>4.5</v>
       </c>
       <c r="F666" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
       <c r="G666" t="s">
-        <v>143</v>
+        <v>239</v>
       </c>
       <c r="H666" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="I666">
-        <v>134</v>
+        <v>209</v>
       </c>
       <c r="J666" t="s">
-        <v>143</v>
+        <v>239</v>
       </c>
     </row>
     <row r="667" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A667" t="s">
-        <v>239</v>
+        <v>436</v>
       </c>
       <c r="B667" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
       <c r="C667">
         <v>3</v>
@@ -19630,104 +19660,92 @@
         <v>4.5</v>
       </c>
       <c r="F667" t="s">
-        <v>545</v>
+        <v>552</v>
       </c>
       <c r="G667" t="s">
-        <v>239</v>
+        <v>436</v>
       </c>
       <c r="H667" t="s">
         <v>556</v>
       </c>
       <c r="I667">
-        <v>209</v>
+        <v>491</v>
       </c>
       <c r="J667" t="s">
-        <v>239</v>
+        <v>901</v>
       </c>
     </row>
     <row r="668" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A668" t="s">
-        <v>436</v>
-      </c>
-      <c r="B668" t="s">
-        <v>528</v>
-      </c>
-      <c r="C668">
-        <v>3</v>
-      </c>
-      <c r="D668" t="s">
-        <v>532</v>
-      </c>
-      <c r="E668">
-        <v>4.5</v>
-      </c>
-      <c r="F668" t="s">
-        <v>552</v>
-      </c>
       <c r="G668" t="s">
-        <v>436</v>
+        <v>798</v>
       </c>
       <c r="H668" t="s">
         <v>556</v>
       </c>
       <c r="I668">
-        <v>491</v>
+        <v>355</v>
       </c>
       <c r="J668" t="s">
-        <v>901</v>
+        <v>798</v>
       </c>
     </row>
     <row r="669" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G669" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="H669" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="I669">
-        <v>355</v>
+        <v>325</v>
       </c>
       <c r="J669" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
     </row>
     <row r="670" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G670" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="H670" t="s">
         <v>557</v>
       </c>
       <c r="I670">
-        <v>325</v>
+        <v>381</v>
       </c>
       <c r="J670" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
     </row>
     <row r="671" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G671" t="s">
-        <v>800</v>
-      </c>
-      <c r="H671" t="s">
-        <v>557</v>
-      </c>
-      <c r="I671">
-        <v>381</v>
-      </c>
-      <c r="J671" t="s">
-        <v>800</v>
+      <c r="A671" t="s">
+        <v>208</v>
+      </c>
+      <c r="B671" t="s">
+        <v>520</v>
+      </c>
+      <c r="C671">
+        <v>2</v>
+      </c>
+      <c r="D671" t="s">
+        <v>534</v>
+      </c>
+      <c r="E671">
+        <v>5</v>
+      </c>
+      <c r="F671" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="672" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A672" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B672" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C672">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D672" t="s">
         <v>534</v>
@@ -19736,360 +19754,360 @@
         <v>5</v>
       </c>
       <c r="F672" t="s">
-        <v>544</v>
+        <v>543</v>
+      </c>
+      <c r="G672" t="s">
+        <v>198</v>
+      </c>
+      <c r="H672" t="s">
+        <v>557</v>
+      </c>
+      <c r="I672">
+        <v>176</v>
+      </c>
+      <c r="J672" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="673" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A673" t="s">
-        <v>198</v>
+        <v>362</v>
       </c>
       <c r="B673" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="C673">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D673" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E673">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F673" t="s">
-        <v>543</v>
-      </c>
-      <c r="G673" t="s">
-        <v>198</v>
-      </c>
-      <c r="H673" t="s">
-        <v>557</v>
-      </c>
-      <c r="I673">
-        <v>176</v>
-      </c>
-      <c r="J673" t="s">
-        <v>198</v>
+        <v>549</v>
       </c>
     </row>
     <row r="674" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A674" t="s">
-        <v>362</v>
+        <v>484</v>
       </c>
       <c r="B674" t="s">
-        <v>525</v>
+        <v>530</v>
       </c>
       <c r="C674">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D674" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="E674">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="F674" t="s">
-        <v>549</v>
+        <v>554</v>
+      </c>
+      <c r="G674" t="s">
+        <v>484</v>
+      </c>
+      <c r="H674" t="s">
+        <v>557</v>
+      </c>
+      <c r="I674">
+        <v>422</v>
+      </c>
+      <c r="J674" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="675" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A675" t="s">
-        <v>484</v>
+        <v>217</v>
       </c>
       <c r="B675" t="s">
-        <v>530</v>
+        <v>520</v>
       </c>
       <c r="C675">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D675" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E675">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="F675" t="s">
-        <v>554</v>
-      </c>
-      <c r="G675" t="s">
-        <v>484</v>
-      </c>
-      <c r="H675" t="s">
-        <v>557</v>
-      </c>
-      <c r="I675">
-        <v>422</v>
-      </c>
-      <c r="J675" t="s">
-        <v>484</v>
+        <v>544</v>
       </c>
     </row>
     <row r="676" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A676" t="s">
-        <v>217</v>
-      </c>
-      <c r="B676" t="s">
-        <v>520</v>
-      </c>
-      <c r="C676">
-        <v>2</v>
-      </c>
-      <c r="D676" t="s">
-        <v>532</v>
-      </c>
-      <c r="E676">
-        <v>4.5</v>
-      </c>
-      <c r="F676" t="s">
-        <v>544</v>
+      <c r="G676" t="s">
+        <v>801</v>
+      </c>
+      <c r="H676" t="s">
+        <v>557</v>
+      </c>
+      <c r="I676">
+        <v>566</v>
+      </c>
+      <c r="J676" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="677" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G677" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="H677" t="s">
         <v>557</v>
       </c>
       <c r="I677">
-        <v>566</v>
+        <v>716</v>
       </c>
       <c r="J677" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
     </row>
     <row r="678" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A678" t="s">
+        <v>505</v>
+      </c>
+      <c r="B678" t="s">
+        <v>531</v>
+      </c>
+      <c r="C678">
+        <v>3</v>
+      </c>
+      <c r="D678" t="s">
+        <v>532</v>
+      </c>
+      <c r="E678">
+        <v>4</v>
+      </c>
+      <c r="F678" t="s">
+        <v>555</v>
+      </c>
       <c r="G678" t="s">
-        <v>802</v>
+        <v>505</v>
       </c>
       <c r="H678" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I678">
-        <v>716</v>
+        <v>685</v>
       </c>
       <c r="J678" t="s">
-        <v>802</v>
+        <v>902</v>
       </c>
     </row>
     <row r="679" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A679" t="s">
-        <v>505</v>
+        <v>294</v>
       </c>
       <c r="B679" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="C679">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D679" t="s">
         <v>532</v>
       </c>
       <c r="E679">
-        <v>4</v>
+        <v>7.5</v>
       </c>
       <c r="F679" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
       <c r="G679" t="s">
-        <v>505</v>
+        <v>294</v>
       </c>
       <c r="H679" t="s">
         <v>556</v>
       </c>
       <c r="I679">
-        <v>685</v>
+        <v>237</v>
       </c>
       <c r="J679" t="s">
-        <v>902</v>
+        <v>294</v>
       </c>
     </row>
     <row r="680" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A680" t="s">
-        <v>294</v>
+        <v>147</v>
       </c>
       <c r="B680" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="C680">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D680" t="s">
         <v>532</v>
       </c>
       <c r="E680">
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="F680" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="G680" t="s">
-        <v>294</v>
+        <v>147</v>
       </c>
       <c r="H680" t="s">
         <v>556</v>
       </c>
       <c r="I680">
-        <v>237</v>
+        <v>527</v>
       </c>
       <c r="J680" t="s">
-        <v>294</v>
+        <v>147</v>
       </c>
     </row>
     <row r="681" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A681" t="s">
-        <v>147</v>
+        <v>469</v>
       </c>
       <c r="B681" t="s">
-        <v>517</v>
+        <v>529</v>
       </c>
       <c r="C681">
         <v>4</v>
       </c>
       <c r="D681" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="E681">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="F681" t="s">
-        <v>541</v>
-      </c>
-      <c r="G681" t="s">
-        <v>147</v>
-      </c>
-      <c r="H681" t="s">
-        <v>556</v>
-      </c>
-      <c r="I681">
-        <v>527</v>
-      </c>
-      <c r="J681" t="s">
-        <v>147</v>
+        <v>553</v>
       </c>
     </row>
     <row r="682" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A682" t="s">
-        <v>469</v>
+        <v>282</v>
       </c>
       <c r="B682" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="C682">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D682" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E682">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="F682" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
     </row>
     <row r="683" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A683" t="s">
-        <v>282</v>
-      </c>
-      <c r="B683" t="s">
-        <v>522</v>
-      </c>
-      <c r="C683">
-        <v>2</v>
-      </c>
-      <c r="D683" t="s">
-        <v>534</v>
-      </c>
-      <c r="E683">
-        <v>5</v>
-      </c>
-      <c r="F683" t="s">
-        <v>546</v>
+      <c r="G683" t="s">
+        <v>803</v>
+      </c>
+      <c r="H683" t="s">
+        <v>558</v>
+      </c>
+      <c r="I683">
+        <v>380</v>
+      </c>
+      <c r="J683" t="s">
+        <v>803</v>
       </c>
     </row>
     <row r="684" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G684" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="H684" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I684">
-        <v>380</v>
+        <v>620</v>
       </c>
       <c r="J684" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
     </row>
     <row r="685" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G685" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="H685" t="s">
         <v>557</v>
       </c>
       <c r="I685">
-        <v>620</v>
+        <v>630</v>
       </c>
       <c r="J685" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
     </row>
     <row r="686" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A686" t="s">
+        <v>263</v>
+      </c>
+      <c r="B686" t="s">
+        <v>522</v>
+      </c>
+      <c r="C686">
+        <v>2</v>
+      </c>
+      <c r="D686" t="s">
+        <v>534</v>
+      </c>
+      <c r="E686">
+        <v>5</v>
+      </c>
+      <c r="F686" t="s">
+        <v>546</v>
+      </c>
       <c r="G686" t="s">
-        <v>805</v>
+        <v>263</v>
       </c>
       <c r="H686" t="s">
         <v>557</v>
       </c>
       <c r="I686">
-        <v>630</v>
+        <v>193</v>
       </c>
       <c r="J686" t="s">
-        <v>805</v>
+        <v>263</v>
       </c>
     </row>
     <row r="687" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A687" t="s">
-        <v>263</v>
+        <v>363</v>
       </c>
       <c r="B687" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="C687">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D687" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E687">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="F687" t="s">
-        <v>546</v>
-      </c>
-      <c r="G687" t="s">
-        <v>263</v>
-      </c>
-      <c r="H687" t="s">
-        <v>557</v>
-      </c>
-      <c r="I687">
-        <v>193</v>
-      </c>
-      <c r="J687" t="s">
-        <v>263</v>
+        <v>549</v>
       </c>
     </row>
     <row r="688" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A688" t="s">
-        <v>363</v>
+        <v>176</v>
       </c>
       <c r="B688" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="C688">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D688" t="s">
         <v>532</v>
@@ -20098,15 +20116,27 @@
         <v>4.5</v>
       </c>
       <c r="F688" t="s">
-        <v>549</v>
+        <v>542</v>
+      </c>
+      <c r="G688" t="s">
+        <v>176</v>
+      </c>
+      <c r="H688" t="s">
+        <v>556</v>
+      </c>
+      <c r="I688">
+        <v>162</v>
+      </c>
+      <c r="J688" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="689" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A689" t="s">
-        <v>176</v>
+        <v>44</v>
       </c>
       <c r="B689" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="C689">
         <v>3</v>
@@ -20118,311 +20148,311 @@
         <v>4.5</v>
       </c>
       <c r="F689" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="G689" t="s">
-        <v>176</v>
+        <v>44</v>
       </c>
       <c r="H689" t="s">
         <v>556</v>
       </c>
       <c r="I689">
-        <v>162</v>
+        <v>38</v>
       </c>
       <c r="J689" t="s">
-        <v>176</v>
+        <v>44</v>
       </c>
     </row>
     <row r="690" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A690" t="s">
-        <v>44</v>
+        <v>158</v>
       </c>
       <c r="B690" t="s">
-        <v>513</v>
+        <v>518</v>
       </c>
       <c r="C690">
         <v>3</v>
       </c>
       <c r="D690" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E690">
         <v>4.5</v>
       </c>
       <c r="F690" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="G690" t="s">
-        <v>44</v>
+        <v>158</v>
       </c>
       <c r="H690" t="s">
-        <v>556</v>
+        <v>815</v>
       </c>
       <c r="I690">
-        <v>38</v>
+        <v>146</v>
       </c>
       <c r="J690" t="s">
-        <v>44</v>
+        <v>158</v>
       </c>
     </row>
     <row r="691" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A691" t="s">
-        <v>158</v>
+        <v>351</v>
       </c>
       <c r="B691" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="C691">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D691" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E691">
         <v>4.5</v>
       </c>
       <c r="F691" t="s">
-        <v>542</v>
+        <v>549</v>
       </c>
       <c r="G691" t="s">
-        <v>158</v>
+        <v>351</v>
       </c>
       <c r="H691" t="s">
-        <v>815</v>
+        <v>556</v>
       </c>
       <c r="I691">
-        <v>146</v>
+        <v>284</v>
       </c>
       <c r="J691" t="s">
-        <v>158</v>
+        <v>351</v>
       </c>
     </row>
     <row r="692" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A692" t="s">
-        <v>351</v>
+        <v>289</v>
       </c>
       <c r="B692" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C692">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D692" t="s">
         <v>532</v>
       </c>
       <c r="E692">
-        <v>4.5</v>
+        <v>6.5</v>
       </c>
       <c r="F692" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="G692" t="s">
-        <v>351</v>
+        <v>289</v>
       </c>
       <c r="H692" t="s">
         <v>556</v>
       </c>
       <c r="I692">
-        <v>284</v>
+        <v>229</v>
       </c>
       <c r="J692" t="s">
-        <v>351</v>
+        <v>289</v>
       </c>
     </row>
     <row r="693" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A693" t="s">
-        <v>289</v>
+        <v>202</v>
       </c>
       <c r="B693" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C693">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D693" t="s">
         <v>532</v>
       </c>
       <c r="E693">
-        <v>6.5</v>
+        <v>4.5</v>
       </c>
       <c r="F693" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="G693" t="s">
-        <v>289</v>
+        <v>202</v>
       </c>
       <c r="H693" t="s">
         <v>556</v>
       </c>
       <c r="I693">
-        <v>229</v>
+        <v>675</v>
       </c>
       <c r="J693" t="s">
-        <v>289</v>
+        <v>202</v>
       </c>
     </row>
     <row r="694" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A694" t="s">
-        <v>202</v>
+        <v>92</v>
       </c>
       <c r="B694" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="C694">
         <v>3</v>
       </c>
       <c r="D694" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="E694">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="F694" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="G694" t="s">
-        <v>202</v>
+        <v>92</v>
       </c>
       <c r="H694" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="I694">
-        <v>675</v>
+        <v>84</v>
       </c>
       <c r="J694" t="s">
-        <v>202</v>
+        <v>92</v>
       </c>
     </row>
     <row r="695" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A695" t="s">
-        <v>92</v>
+        <v>479</v>
       </c>
       <c r="B695" t="s">
-        <v>515</v>
+        <v>530</v>
       </c>
       <c r="C695">
         <v>3</v>
       </c>
       <c r="D695" t="s">
+        <v>532</v>
+      </c>
+      <c r="E695">
+        <v>4.5</v>
+      </c>
+      <c r="F695" t="s">
+        <v>554</v>
+      </c>
+      <c r="G695" t="s">
+        <v>479</v>
+      </c>
+      <c r="H695" t="s">
+        <v>556</v>
+      </c>
+      <c r="I695">
+        <v>418</v>
+      </c>
+      <c r="J695" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="696" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G696" t="s">
+        <v>806</v>
+      </c>
+      <c r="H696" t="s">
+        <v>815</v>
+      </c>
+      <c r="I696">
+        <v>480</v>
+      </c>
+      <c r="J696" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="697" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A697" t="s">
+        <v>253</v>
+      </c>
+      <c r="B697" t="s">
+        <v>521</v>
+      </c>
+      <c r="C697">
+        <v>3</v>
+      </c>
+      <c r="D697" t="s">
+        <v>532</v>
+      </c>
+      <c r="E697">
+        <v>4.5</v>
+      </c>
+      <c r="F697" t="s">
+        <v>545</v>
+      </c>
+      <c r="G697" t="s">
+        <v>253</v>
+      </c>
+      <c r="H697" t="s">
+        <v>556</v>
+      </c>
+      <c r="I697">
+        <v>220</v>
+      </c>
+      <c r="J697" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="698" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G698" t="s">
+        <v>807</v>
+      </c>
+      <c r="H698" t="s">
+        <v>558</v>
+      </c>
+      <c r="I698">
+        <v>47</v>
+      </c>
+      <c r="J698" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="699" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A699" t="s">
+        <v>246</v>
+      </c>
+      <c r="B699" t="s">
+        <v>521</v>
+      </c>
+      <c r="C699">
+        <v>3</v>
+      </c>
+      <c r="D699" t="s">
         <v>534</v>
       </c>
-      <c r="E695">
-        <v>5.5</v>
-      </c>
-      <c r="F695" t="s">
-        <v>539</v>
-      </c>
-      <c r="G695" t="s">
-        <v>92</v>
-      </c>
-      <c r="H695" t="s">
-        <v>557</v>
-      </c>
-      <c r="I695">
-        <v>84</v>
-      </c>
-      <c r="J695" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="696" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A696" t="s">
-        <v>479</v>
-      </c>
-      <c r="B696" t="s">
-        <v>530</v>
-      </c>
-      <c r="C696">
-        <v>3</v>
-      </c>
-      <c r="D696" t="s">
-        <v>532</v>
-      </c>
-      <c r="E696">
-        <v>4.5</v>
-      </c>
-      <c r="F696" t="s">
-        <v>554</v>
-      </c>
-      <c r="G696" t="s">
-        <v>479</v>
-      </c>
-      <c r="H696" t="s">
-        <v>556</v>
-      </c>
-      <c r="I696">
-        <v>418</v>
-      </c>
-      <c r="J696" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="697" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G697" t="s">
-        <v>806</v>
-      </c>
-      <c r="H697" t="s">
-        <v>815</v>
-      </c>
-      <c r="I697">
-        <v>480</v>
-      </c>
-      <c r="J697" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="698" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A698" t="s">
-        <v>253</v>
-      </c>
-      <c r="B698" t="s">
-        <v>521</v>
-      </c>
-      <c r="C698">
-        <v>3</v>
-      </c>
-      <c r="D698" t="s">
-        <v>532</v>
-      </c>
-      <c r="E698">
-        <v>4.5</v>
-      </c>
-      <c r="F698" t="s">
+      <c r="E699">
+        <v>5</v>
+      </c>
+      <c r="F699" t="s">
         <v>545</v>
       </c>
-      <c r="G698" t="s">
-        <v>253</v>
-      </c>
-      <c r="H698" t="s">
-        <v>556</v>
-      </c>
-      <c r="I698">
-        <v>220</v>
-      </c>
-      <c r="J698" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="699" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G699" t="s">
-        <v>807</v>
+        <v>246</v>
       </c>
       <c r="H699" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I699">
-        <v>47</v>
+        <v>216</v>
       </c>
       <c r="J699" t="s">
-        <v>903</v>
+        <v>246</v>
       </c>
     </row>
     <row r="700" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A700" t="s">
-        <v>246</v>
+        <v>166</v>
       </c>
       <c r="B700" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="C700">
         <v>3</v>
@@ -20431,82 +20461,82 @@
         <v>534</v>
       </c>
       <c r="E700">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F700" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="G700" t="s">
-        <v>246</v>
+        <v>166</v>
       </c>
       <c r="H700" t="s">
         <v>557</v>
       </c>
       <c r="I700">
-        <v>216</v>
+        <v>154</v>
       </c>
       <c r="J700" t="s">
-        <v>246</v>
+        <v>166</v>
       </c>
     </row>
     <row r="701" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A701" t="s">
-        <v>166</v>
+        <v>82</v>
       </c>
       <c r="B701" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="C701">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D701" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E701">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F701" t="s">
-        <v>542</v>
-      </c>
-      <c r="G701" t="s">
-        <v>166</v>
-      </c>
-      <c r="H701" t="s">
-        <v>557</v>
-      </c>
-      <c r="I701">
-        <v>154</v>
-      </c>
-      <c r="J701" t="s">
-        <v>166</v>
+        <v>538</v>
       </c>
     </row>
     <row r="702" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A702" t="s">
-        <v>82</v>
+        <v>169</v>
       </c>
       <c r="B702" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="C702">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D702" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="E702">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F702" t="s">
-        <v>538</v>
+        <v>542</v>
+      </c>
+      <c r="G702" t="s">
+        <v>169</v>
+      </c>
+      <c r="H702" t="s">
+        <v>557</v>
+      </c>
+      <c r="I702">
+        <v>386</v>
+      </c>
+      <c r="J702" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="703" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A703" t="s">
-        <v>169</v>
+        <v>432</v>
       </c>
       <c r="B703" t="s">
-        <v>518</v>
+        <v>528</v>
       </c>
       <c r="C703">
         <v>3</v>
@@ -20515,250 +20545,250 @@
         <v>534</v>
       </c>
       <c r="E703">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="F703" t="s">
-        <v>542</v>
-      </c>
-      <c r="G703" t="s">
-        <v>169</v>
-      </c>
-      <c r="H703" t="s">
-        <v>557</v>
-      </c>
-      <c r="I703">
-        <v>386</v>
-      </c>
-      <c r="J703" t="s">
-        <v>169</v>
+        <v>552</v>
       </c>
     </row>
     <row r="704" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A704" t="s">
-        <v>432</v>
-      </c>
-      <c r="B704" t="s">
-        <v>528</v>
-      </c>
-      <c r="C704">
-        <v>3</v>
-      </c>
-      <c r="D704" t="s">
-        <v>534</v>
-      </c>
-      <c r="E704">
+      <c r="G704" t="s">
+        <v>808</v>
+      </c>
+      <c r="H704" t="s">
+        <v>815</v>
+      </c>
+      <c r="I704">
+        <v>114</v>
+      </c>
+      <c r="J704" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="705" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A705" t="s">
+        <v>31</v>
+      </c>
+      <c r="B705" t="s">
+        <v>512</v>
+      </c>
+      <c r="C705">
+        <v>4</v>
+      </c>
+      <c r="D705" t="s">
+        <v>532</v>
+      </c>
+      <c r="E705">
         <v>4.5</v>
       </c>
-      <c r="F704" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="705" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F705" t="s">
+        <v>536</v>
+      </c>
       <c r="G705" t="s">
-        <v>808</v>
+        <v>31</v>
       </c>
       <c r="H705" t="s">
-        <v>815</v>
+        <v>556</v>
       </c>
       <c r="I705">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="J705" t="s">
-        <v>808</v>
+        <v>31</v>
       </c>
     </row>
     <row r="706" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A706" t="s">
-        <v>31</v>
-      </c>
-      <c r="B706" t="s">
-        <v>512</v>
-      </c>
-      <c r="C706">
-        <v>4</v>
-      </c>
-      <c r="D706" t="s">
-        <v>532</v>
-      </c>
-      <c r="E706">
-        <v>4.5</v>
-      </c>
-      <c r="F706" t="s">
-        <v>536</v>
-      </c>
       <c r="G706" t="s">
-        <v>31</v>
+        <v>809</v>
       </c>
       <c r="H706" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="I706">
-        <v>27</v>
+        <v>347</v>
       </c>
       <c r="J706" t="s">
-        <v>31</v>
+        <v>809</v>
       </c>
     </row>
     <row r="707" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G707" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="H707" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I707">
-        <v>347</v>
+        <v>387</v>
       </c>
       <c r="J707" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
     </row>
     <row r="708" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A708" t="s">
+        <v>490</v>
+      </c>
+      <c r="B708" t="s">
+        <v>531</v>
+      </c>
+      <c r="C708">
+        <v>3</v>
+      </c>
+      <c r="D708" t="s">
+        <v>532</v>
+      </c>
+      <c r="E708">
+        <v>4.5</v>
+      </c>
+      <c r="F708" t="s">
+        <v>555</v>
+      </c>
       <c r="G708" t="s">
-        <v>810</v>
+        <v>490</v>
       </c>
       <c r="H708" t="s">
         <v>556</v>
       </c>
       <c r="I708">
-        <v>387</v>
+        <v>428</v>
       </c>
       <c r="J708" t="s">
-        <v>810</v>
+        <v>490</v>
       </c>
     </row>
     <row r="709" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A709" t="s">
-        <v>490</v>
+        <v>441</v>
       </c>
       <c r="B709" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C709">
         <v>3</v>
       </c>
       <c r="D709" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E709">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="F709" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="G709" t="s">
-        <v>490</v>
+        <v>441</v>
       </c>
       <c r="H709" t="s">
-        <v>556</v>
+        <v>815</v>
       </c>
       <c r="I709">
-        <v>428</v>
+        <v>641</v>
       </c>
       <c r="J709" t="s">
-        <v>490</v>
+        <v>441</v>
       </c>
     </row>
     <row r="710" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A710" t="s">
-        <v>441</v>
+        <v>405</v>
       </c>
       <c r="B710" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C710">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D710" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="E710">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F710" t="s">
-        <v>552</v>
-      </c>
-      <c r="G710" t="s">
-        <v>441</v>
-      </c>
-      <c r="H710" t="s">
-        <v>815</v>
-      </c>
-      <c r="I710">
-        <v>641</v>
-      </c>
-      <c r="J710" t="s">
-        <v>441</v>
+        <v>551</v>
       </c>
     </row>
     <row r="711" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A711" t="s">
-        <v>405</v>
-      </c>
-      <c r="B711" t="s">
-        <v>527</v>
-      </c>
-      <c r="C711">
-        <v>2</v>
-      </c>
-      <c r="D711" t="s">
-        <v>534</v>
-      </c>
-      <c r="E711">
-        <v>5</v>
-      </c>
-      <c r="F711" t="s">
-        <v>551</v>
+      <c r="G711" t="s">
+        <v>811</v>
+      </c>
+      <c r="H711" t="s">
+        <v>556</v>
+      </c>
+      <c r="I711">
+        <v>410</v>
+      </c>
+      <c r="J711" t="s">
+        <v>811</v>
       </c>
     </row>
     <row r="712" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G712" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="H712" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="I712">
-        <v>410</v>
+        <v>700</v>
       </c>
       <c r="J712" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
     </row>
     <row r="713" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G713" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="H713" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I713">
-        <v>700</v>
+        <v>226</v>
       </c>
       <c r="J713" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="714" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A714" t="s">
+        <v>431</v>
+      </c>
+      <c r="B714" t="s">
+        <v>528</v>
+      </c>
+      <c r="C714">
+        <v>3</v>
+      </c>
+      <c r="D714" t="s">
+        <v>532</v>
+      </c>
+      <c r="E714">
+        <v>4</v>
+      </c>
+      <c r="F714" t="s">
+        <v>552</v>
+      </c>
       <c r="G714" t="s">
-        <v>813</v>
+        <v>431</v>
       </c>
       <c r="H714" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I714">
-        <v>226</v>
+        <v>546</v>
       </c>
       <c r="J714" t="s">
-        <v>813</v>
+        <v>431</v>
       </c>
     </row>
     <row r="715" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A715" t="s">
-        <v>431</v>
+        <v>196</v>
       </c>
       <c r="B715" t="s">
-        <v>528</v>
+        <v>519</v>
       </c>
       <c r="C715">
         <v>3</v>
@@ -20767,30 +20797,30 @@
         <v>532</v>
       </c>
       <c r="E715">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="F715" t="s">
-        <v>552</v>
+        <v>543</v>
       </c>
       <c r="G715" t="s">
-        <v>431</v>
+        <v>196</v>
       </c>
       <c r="H715" t="s">
         <v>556</v>
       </c>
       <c r="I715">
-        <v>546</v>
+        <v>175</v>
       </c>
       <c r="J715" t="s">
-        <v>431</v>
+        <v>196</v>
       </c>
     </row>
     <row r="716" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A716" t="s">
-        <v>196</v>
+        <v>510</v>
       </c>
       <c r="B716" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="C716">
         <v>3</v>
@@ -20799,50 +20829,50 @@
         <v>532</v>
       </c>
       <c r="E716">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="F716" t="s">
-        <v>543</v>
-      </c>
-      <c r="G716" t="s">
-        <v>196</v>
-      </c>
-      <c r="H716" t="s">
-        <v>556</v>
-      </c>
-      <c r="I716">
-        <v>175</v>
-      </c>
-      <c r="J716" t="s">
-        <v>196</v>
+        <v>555</v>
       </c>
     </row>
     <row r="717" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A717" t="s">
-        <v>510</v>
+        <v>95</v>
       </c>
       <c r="B717" t="s">
-        <v>531</v>
+        <v>515</v>
       </c>
       <c r="C717">
         <v>3</v>
       </c>
       <c r="D717" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="E717">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="F717" t="s">
-        <v>555</v>
+        <v>539</v>
+      </c>
+      <c r="G717" t="s">
+        <v>95</v>
+      </c>
+      <c r="H717" t="s">
+        <v>557</v>
+      </c>
+      <c r="I717">
+        <v>524</v>
+      </c>
+      <c r="J717" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="718" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A718" t="s">
-        <v>95</v>
+        <v>240</v>
       </c>
       <c r="B718" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="C718">
         <v>3</v>
@@ -20851,117 +20881,85 @@
         <v>534</v>
       </c>
       <c r="E718">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="F718" t="s">
-        <v>539</v>
+        <v>545</v>
       </c>
       <c r="G718" t="s">
-        <v>95</v>
+        <v>240</v>
       </c>
       <c r="H718" t="s">
         <v>557</v>
       </c>
       <c r="I718">
-        <v>524</v>
+        <v>210</v>
       </c>
       <c r="J718" t="s">
-        <v>95</v>
+        <v>240</v>
       </c>
     </row>
     <row r="719" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A719" t="s">
-        <v>240</v>
+        <v>460</v>
       </c>
       <c r="B719" t="s">
-        <v>521</v>
+        <v>529</v>
       </c>
       <c r="C719">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D719" t="s">
         <v>534</v>
       </c>
       <c r="E719">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="F719" t="s">
-        <v>545</v>
+        <v>553</v>
       </c>
       <c r="G719" t="s">
-        <v>240</v>
+        <v>460</v>
       </c>
       <c r="H719" t="s">
         <v>557</v>
       </c>
       <c r="I719">
-        <v>210</v>
+        <v>70</v>
       </c>
       <c r="J719" t="s">
-        <v>240</v>
+        <v>460</v>
       </c>
     </row>
     <row r="720" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A720" t="s">
-        <v>460</v>
+        <v>324</v>
       </c>
       <c r="B720" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="C720">
+        <v>5</v>
+      </c>
+      <c r="D720" t="s">
+        <v>533</v>
+      </c>
+      <c r="E720">
         <v>4</v>
       </c>
-      <c r="D720" t="s">
-        <v>534</v>
-      </c>
-      <c r="E720">
-        <v>5</v>
-      </c>
       <c r="F720" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="G720" t="s">
-        <v>460</v>
+        <v>324</v>
       </c>
       <c r="H720" t="s">
-        <v>557</v>
+        <v>815</v>
       </c>
       <c r="I720">
-        <v>70</v>
+        <v>260</v>
       </c>
       <c r="J720" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="721" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A721" t="s">
-        <v>324</v>
-      </c>
-      <c r="B721" t="s">
-        <v>524</v>
-      </c>
-      <c r="C721">
-        <v>5</v>
-      </c>
-      <c r="D721" t="s">
-        <v>533</v>
-      </c>
-      <c r="E721">
-        <v>4</v>
-      </c>
-      <c r="F721" t="s">
-        <v>548</v>
-      </c>
-      <c r="G721" t="s">
-        <v>324</v>
-      </c>
-      <c r="H721" t="s">
-        <v>815</v>
-      </c>
-      <c r="I721">
-        <v>260</v>
-      </c>
-      <c r="J721" t="s">
         <v>324</v>
       </c>
     </row>

</xml_diff>